<commit_message>
added state and state+year level data files, created us maps with plotly
</commit_message>
<xml_diff>
--- a/data/census_population_and_voting.xlsx
+++ b/data/census_population_and_voting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendallkikkawa/Documents/BAPP/GFI_rancher_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83157879-AC60-BE4D-A07A-32451C71604C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84A45E2-5038-1540-8CD4-9F2904263297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E827D3EE-5171-E046-9EF1-B82E81DAECCC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{E827D3EE-5171-E046-9EF1-B82E81DAECCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Total_population</t>
-  </si>
-  <si>
     <t>Total_Registered</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>Total_Citizen_Population</t>
+  </si>
+  <si>
+    <t>Total_Population</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,43 +637,43 @@
         <v>51</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>